<commit_message>
konvertert siste rest til pdf
</commit_message>
<xml_diff>
--- a/Dokumentasjon/vedlegg/04. Risikoplan.xlsx
+++ b/Dokumentasjon/vedlegg/04. Risikoplan.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="466" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="466"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Ark 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -149,11 +148,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -162,22 +158,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -185,8 +166,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <i val="true"/>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -216,7 +197,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -224,65 +205,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -341,33 +285,329 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A6" view="normal" windowProtection="false" workbookViewId="0" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100">
-      <selection activeCell="D5" activeCellId="0" pane="topLeft" sqref="D5"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScale="55" zoomScaleNormal="60" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="17.1326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.984693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="70.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="17.1326530612245"/>
+    <col min="1" max="1" width="26.140625"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="72" customWidth="1"/>
+    <col min="6" max="6" width="70.5703125"/>
+    <col min="7" max="1025" width="17.140625"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -381,7 +621,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="2">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -389,7 +629,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="3">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -409,18 +649,18 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="5">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="5">
         <v>0.5</v>
       </c>
-      <c r="D4" s="5" t="n">
-        <f aca="false">B4*C4</f>
+      <c r="D4" s="5">
+        <f t="shared" ref="D4:D14" si="0">B4*C4</f>
         <v>3.5</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -430,18 +670,18 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="5">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="5">
         <v>0.4</v>
       </c>
-      <c r="D5" s="5" t="n">
-        <f aca="false">B5*C5</f>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -451,18 +691,18 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+    <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="5">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="5">
         <v>0.5</v>
       </c>
-      <c r="D6" s="5" t="n">
-        <f aca="false">B6*C6</f>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -472,18 +712,18 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
+    <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="5">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="5">
         <v>0.5</v>
       </c>
-      <c r="D7" s="5" t="n">
-        <f aca="false">B7*C7</f>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -493,18 +733,18 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="5">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="5">
         <v>0.5</v>
       </c>
-      <c r="D8" s="5" t="n">
-        <f aca="false">B8*C8</f>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -514,19 +754,19 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+    <row r="9" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="5">
         <v>0.4</v>
       </c>
-      <c r="D9" s="5" t="n">
-        <f aca="false">B9*C9</f>
-        <v>2.4</v>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>25</v>
@@ -535,18 +775,18 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+    <row r="10" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="5">
         <v>0.3</v>
       </c>
-      <c r="D10" s="5" t="n">
-        <f aca="false">B10*C10</f>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
         <v>2.1</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -556,18 +796,18 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+    <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="5">
         <v>0.3</v>
       </c>
-      <c r="D11" s="5" t="n">
-        <f aca="false">B11*C11</f>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
         <v>2.1</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -577,18 +817,18 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="12">
+    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="5">
         <v>4</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="5">
         <v>0.5</v>
       </c>
-      <c r="D12" s="5" t="n">
-        <f aca="false">B12*C12</f>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -598,18 +838,18 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="13">
+    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="5">
         <v>5</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="5">
         <v>0.3</v>
       </c>
-      <c r="D13" s="5" t="n">
-        <f aca="false">B13*C13</f>
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -619,18 +859,18 @@
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+    <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="5">
         <v>5</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="5">
         <v>0.3</v>
       </c>
-      <c r="D14" s="5" t="n">
-        <f aca="false">B14*C14</f>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -640,7 +880,7 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="17">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -648,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="19">
+    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
@@ -668,18 +908,18 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="20">
+    <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="5" t="n">
+      <c r="B20" s="5">
         <v>8</v>
       </c>
-      <c r="C20" s="5" t="n">
+      <c r="C20" s="5">
         <v>0.5</v>
       </c>
-      <c r="D20" s="5" t="n">
-        <f aca="false">B20*C20</f>
+      <c r="D20" s="5">
+        <f t="shared" ref="D20:D30" si="1">B20*C20</f>
         <v>4</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -689,18 +929,18 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="21">
+    <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5" t="n">
+      <c r="B21" s="5">
         <v>7</v>
       </c>
-      <c r="C21" s="5" t="n">
+      <c r="C21" s="5">
         <v>0.5</v>
       </c>
-      <c r="D21" s="5" t="n">
-        <f aca="false">B21*C21</f>
+      <c r="D21" s="5">
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -710,18 +950,18 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="22">
+    <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="5" t="n">
+      <c r="B22" s="5">
         <v>8</v>
       </c>
-      <c r="C22" s="5" t="n">
+      <c r="C22" s="5">
         <v>0.4</v>
       </c>
-      <c r="D22" s="5" t="n">
-        <f aca="false">B22*C22</f>
+      <c r="D22" s="5">
+        <f t="shared" si="1"/>
         <v>3.2</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -731,18 +971,18 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="23">
+    <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="5" t="n">
+      <c r="B23" s="5">
         <v>6</v>
       </c>
-      <c r="C23" s="5" t="n">
+      <c r="C23" s="5">
         <v>0.5</v>
       </c>
-      <c r="D23" s="5" t="n">
-        <f aca="false">B23*C23</f>
+      <c r="D23" s="5">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -752,19 +992,19 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="24">
+    <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="5" t="n">
+      <c r="B24" s="5">
         <v>7</v>
       </c>
-      <c r="C24" s="5" t="n">
+      <c r="C24" s="5">
         <v>0.4</v>
       </c>
-      <c r="D24" s="5" t="n">
-        <f aca="false">B24*C24</f>
-        <v>2.8</v>
+      <c r="D24" s="5">
+        <f t="shared" si="1"/>
+        <v>2.8000000000000003</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>16</v>
@@ -773,18 +1013,18 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="25">
+    <row r="25" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="5" t="n">
+      <c r="B25" s="5">
         <v>5</v>
       </c>
-      <c r="C25" s="5" t="n">
+      <c r="C25" s="5">
         <v>0.5</v>
       </c>
-      <c r="D25" s="5" t="n">
-        <f aca="false">B25*C25</f>
+      <c r="D25" s="5">
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -794,18 +1034,18 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="26">
+    <row r="26" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="5" t="n">
+      <c r="B26" s="5">
         <v>7</v>
       </c>
-      <c r="C26" s="5" t="n">
+      <c r="C26" s="5">
         <v>0.3</v>
       </c>
-      <c r="D26" s="5" t="n">
-        <f aca="false">B26*C26</f>
+      <c r="D26" s="5">
+        <f t="shared" si="1"/>
         <v>2.1</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -815,18 +1055,18 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="27">
+    <row r="27" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="5" t="n">
+      <c r="B27" s="5">
         <v>7</v>
       </c>
-      <c r="C27" s="5" t="n">
+      <c r="C27" s="5">
         <v>0.3</v>
       </c>
-      <c r="D27" s="5" t="n">
-        <f aca="false">B27*C27</f>
+      <c r="D27" s="5">
+        <f t="shared" si="1"/>
         <v>2.1</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -836,18 +1076,18 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="28">
+    <row r="28" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="5" t="n">
+      <c r="B28" s="5">
         <v>7</v>
       </c>
-      <c r="C28" s="5" t="n">
+      <c r="C28" s="5">
         <v>0.3</v>
       </c>
-      <c r="D28" s="5" t="n">
-        <f aca="false">B28*C28</f>
+      <c r="D28" s="5">
+        <f t="shared" si="1"/>
         <v>2.1</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -857,18 +1097,18 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="29">
+    <row r="29" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="5" t="n">
+      <c r="B29" s="5">
         <v>5</v>
       </c>
-      <c r="C29" s="5" t="n">
+      <c r="C29" s="5">
         <v>0.2</v>
       </c>
-      <c r="D29" s="5" t="n">
-        <f aca="false">B29*C29</f>
+      <c r="D29" s="5">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -878,18 +1118,18 @@
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="30">
+    <row r="30" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="5" t="n">
+      <c r="B30" s="5">
         <v>5</v>
       </c>
-      <c r="C30" s="5" t="n">
+      <c r="C30" s="5">
         <v>0.2</v>
       </c>
-      <c r="D30" s="5" t="n">
-        <f aca="false">B30*C30</f>
+      <c r="D30" s="5">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -899,7 +1139,7 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="33">
+    <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -907,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="35">
+    <row r="35" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>3</v>
       </c>
@@ -927,18 +1167,18 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="36">
+    <row r="36" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="5" t="n">
+      <c r="B36" s="5">
         <v>9</v>
       </c>
-      <c r="C36" s="5" t="n">
+      <c r="C36" s="5">
         <v>0.4</v>
       </c>
-      <c r="D36" s="5" t="n">
-        <f aca="false">B36*C36</f>
+      <c r="D36" s="5">
+        <f t="shared" ref="D36:D46" si="2">B36*C36</f>
         <v>3.6</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -948,18 +1188,18 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="37">
+    <row r="37" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="5" t="n">
+      <c r="B37" s="5">
         <v>9</v>
       </c>
-      <c r="C37" s="5" t="n">
+      <c r="C37" s="5">
         <v>0.4</v>
       </c>
-      <c r="D37" s="5" t="n">
-        <f aca="false">B37*C37</f>
+      <c r="D37" s="5">
+        <f t="shared" si="2"/>
         <v>3.6</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -969,18 +1209,18 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="38">
+    <row r="38" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="5" t="n">
+      <c r="B38" s="5">
         <v>8</v>
       </c>
-      <c r="C38" s="5" t="n">
+      <c r="C38" s="5">
         <v>0.4</v>
       </c>
-      <c r="D38" s="5" t="n">
-        <f aca="false">B38*C38</f>
+      <c r="D38" s="5">
+        <f t="shared" si="2"/>
         <v>3.2</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -990,19 +1230,19 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="39">
+    <row r="39" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="5" t="n">
+      <c r="B39" s="5">
         <v>7</v>
       </c>
-      <c r="C39" s="5" t="n">
+      <c r="C39" s="5">
         <v>0.4</v>
       </c>
-      <c r="D39" s="5" t="n">
-        <f aca="false">B39*C39</f>
-        <v>2.8</v>
+      <c r="D39" s="5">
+        <f t="shared" si="2"/>
+        <v>2.8000000000000003</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>31</v>
@@ -1011,18 +1251,18 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="40">
+    <row r="40" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="5" t="n">
+      <c r="B40" s="5">
         <v>7</v>
       </c>
-      <c r="C40" s="5" t="n">
+      <c r="C40" s="5">
         <v>0.3</v>
       </c>
-      <c r="D40" s="5" t="n">
-        <f aca="false">B40*C40</f>
+      <c r="D40" s="5">
+        <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -1032,18 +1272,18 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="41">
+    <row r="41" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="5" t="n">
+      <c r="B41" s="5">
         <v>7</v>
       </c>
-      <c r="C41" s="5" t="n">
+      <c r="C41" s="5">
         <v>0.3</v>
       </c>
-      <c r="D41" s="5" t="n">
-        <f aca="false">B41*C41</f>
+      <c r="D41" s="5">
+        <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -1053,18 +1293,18 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="42">
+    <row r="42" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="5" t="n">
+      <c r="B42" s="5">
         <v>5</v>
       </c>
-      <c r="C42" s="5" t="n">
+      <c r="C42" s="5">
         <v>0.3</v>
       </c>
-      <c r="D42" s="5" t="n">
-        <f aca="false">B42*C42</f>
+      <c r="D42" s="5">
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -1074,18 +1314,18 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="43">
+    <row r="43" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="5" t="n">
+      <c r="B43" s="5">
         <v>5</v>
       </c>
-      <c r="C43" s="5" t="n">
+      <c r="C43" s="5">
         <v>0.3</v>
       </c>
-      <c r="D43" s="5" t="n">
-        <f aca="false">B43*C43</f>
+      <c r="D43" s="5">
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1095,18 +1335,18 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="44">
+    <row r="44" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="5" t="n">
+      <c r="B44" s="5">
         <v>4</v>
       </c>
-      <c r="C44" s="5" t="n">
+      <c r="C44" s="5">
         <v>0.3</v>
       </c>
-      <c r="D44" s="5" t="n">
-        <f aca="false">B44*C44</f>
+      <c r="D44" s="5">
+        <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1116,19 +1356,19 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="45">
+    <row r="45" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="5" t="n">
+      <c r="B45" s="5">
         <v>6</v>
       </c>
-      <c r="C45" s="5" t="n">
+      <c r="C45" s="5">
         <v>0.2</v>
       </c>
-      <c r="D45" s="5" t="n">
-        <f aca="false">B45*C45</f>
-        <v>1.2</v>
+      <c r="D45" s="5">
+        <f t="shared" si="2"/>
+        <v>1.2000000000000002</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>36</v>
@@ -1137,19 +1377,19 @@
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="46">
+    <row r="46" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="5" t="n">
+      <c r="B46" s="5">
         <v>6</v>
       </c>
-      <c r="C46" s="5" t="n">
+      <c r="C46" s="5">
         <v>0.2</v>
       </c>
-      <c r="D46" s="5" t="n">
-        <f aca="false">B46*C46</f>
-        <v>1.2</v>
+      <c r="D46" s="5">
+        <f t="shared" si="2"/>
+        <v>1.2000000000000002</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>39</v>
@@ -1159,12 +1399,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>